<commit_message>
12/02/2019 : Remplacement des gros boutons par des plus petits
Impact :
	Mise à jour du fichier Excel FrogINT_BOM_V03-Commit-22-01-2019_RFQ_RS.xlsx suite à la mise à jour de la BOM (Attention pour les chiffrage en cours)
	Création des fichiers sources mécaniques pour ce nouveau Switch_PTS810SJG250SMTRLFS
	Mise à jour des références des librairies (pointeur).
	Déplacement partiel de la librairie SamacSys_Parts directement dans la "racine" du projet (et non plus dans l'arborescence C: etc.)
</commit_message>
<xml_diff>
--- a/04_Electronique/FrogINT_PCBProto_V1811062154/FrogINT_BOM_V03-Commit-22-01-2019_RFQ_RS.xlsx
+++ b/04_Electronique/FrogINT_PCBProto_V1811062154/FrogINT_BOM_V03-Commit-22-01-2019_RFQ_RS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21231"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FrogINT\FrogINTHardware\04_Electronique\FrogINT_PCBProto_V1811062154\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F196CC0-5D9E-482F-8D2B-DDD7AD891534}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9970651-932A-432E-90C1-84A2A7851E67}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="A_Lire" sheetId="3" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="167">
   <si>
     <t>Component,Description,Part,References,Value,Footprint,Quantity Per PCB,Datasheet,Manufacturer_Name,Height,Manufacturer_Part_Number,Mouser Part Number,Mouser Price/Stock,RS Price/Stock,RS Part Number</t>
   </si>
@@ -502,9 +502,6 @@
     <t>121-889</t>
   </si>
   <si>
-    <t>758-2076</t>
-  </si>
-  <si>
     <t>PCB</t>
   </si>
   <si>
@@ -518,6 +515,15 @@
   </si>
   <si>
     <t>814-1764</t>
+  </si>
+  <si>
+    <t>Bouton</t>
+  </si>
+  <si>
+    <t>135-9492</t>
+  </si>
+  <si>
+    <t>PTS810 SJG 250 SMTR LFS</t>
   </si>
 </sst>
 </file>
@@ -526,9 +532,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -644,6 +650,13 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -972,7 +985,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1016,23 +1029,25 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="42" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="33" borderId="10" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="42" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="33" borderId="10" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="43"/>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="44">
     <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20 % - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20 % - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1062,6 +1077,7 @@
     <cellStyle name="Cellule liée" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Entrée" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Insatisfaisant" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Lien hypertexte" xfId="43" builtinId="8"/>
     <cellStyle name="Monétaire" xfId="42" builtinId="4"/>
     <cellStyle name="Neutre" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2186,7 +2202,7 @@
   <dimension ref="A1:T28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J2:J21"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2793,57 +2809,39 @@
       <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" s="1"/>
+      <c r="B16" s="1" t="s">
+        <v>164</v>
+      </c>
       <c r="C16" s="1" t="s">
-        <v>101</v>
+        <v>166</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>102</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>103</v>
+        <v>166</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>103</v>
+        <v>166</v>
       </c>
       <c r="G16" s="1">
         <v>2</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="I16" s="4">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="J16" s="5">
-        <v>0.33100000000000002</v>
+        <v>0.28499999999999998</v>
       </c>
       <c r="K16" s="6">
         <f t="shared" si="0"/>
-        <v>3.31</v>
+        <v>5.6999999999999993</v>
       </c>
       <c r="L16" s="8"/>
-      <c r="M16" t="s">
-        <v>104</v>
-      </c>
-      <c r="N16" t="s">
-        <v>105</v>
-      </c>
-      <c r="P16" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>106</v>
-      </c>
-      <c r="R16" t="s">
-        <v>107</v>
-      </c>
-      <c r="S16" t="s">
-        <v>108</v>
-      </c>
-      <c r="T16" t="s">
-        <v>109</v>
-      </c>
+      <c r="M16" s="11"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
@@ -2873,7 +2871,7 @@
         <v>0</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
@@ -2897,7 +2895,7 @@
         <v>1</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I18" s="4">
         <v>2</v>
@@ -2934,7 +2932,7 @@
         <v>1</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I19" s="4">
         <v>10</v>
@@ -2974,7 +2972,7 @@
         <v>1</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I20" s="4">
         <v>20</v>
@@ -3014,7 +3012,7 @@
         <v>1</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I21" s="4">
         <v>5</v>
@@ -3034,7 +3032,7 @@
       </c>
       <c r="K23" s="10">
         <f>SUM(K2:K21)</f>
-        <v>58.61</v>
+        <v>61</v>
       </c>
       <c r="L23" s="3"/>
     </row>
@@ -3056,7 +3054,7 @@
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="K28" s="3">
         <f>K23/K26</f>
-        <v>11.722</v>
+        <v>12.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>